<commit_message>
Updated Excel sheet for sprint 4
</commit_message>
<xml_diff>
--- a/khrwhjvtReport.xlsx
+++ b/khrwhjvtReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27426"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vardaantyagi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Harish7KJ/Desktop/ssw555-master-7/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="260" yWindow="460" windowWidth="22740" windowHeight="14420" tabRatio="500" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="217">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1098,11 +1098,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1730809872"/>
-        <c:axId val="-1730807552"/>
+        <c:axId val="-1204079376"/>
+        <c:axId val="-1204078016"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1730809872"/>
+        <c:axId val="-1204079376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1112,14 +1112,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1730807552"/>
+        <c:crossAx val="-1204078016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1730807552"/>
+        <c:axId val="-1204078016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1130,7 +1130,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1730809872"/>
+        <c:crossAx val="-1204079376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1223,11 +1223,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1730766688"/>
-        <c:axId val="-1730763936"/>
+        <c:axId val="-1206292736"/>
+        <c:axId val="-1177488352"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1730766688"/>
+        <c:axId val="-1206292736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,14 +1237,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1730763936"/>
+        <c:crossAx val="-1177488352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1730763936"/>
+        <c:axId val="-1177488352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1255,7 +1255,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1730766688"/>
+        <c:crossAx val="-1206292736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1292,7 +1292,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1330,7 +1330,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1405,7 +1405,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1470,7 +1470,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1539,7 +1539,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1609,7 +1609,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1678,7 +1678,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1748,7 +1748,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3682,7 +3682,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4011,10 +4011,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4110,6 +4110,15 @@
       <c r="F4">
         <v>45</v>
       </c>
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4" s="19">
+        <v>41583</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
@@ -4130,6 +4139,15 @@
       <c r="F5">
         <v>45</v>
       </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+      <c r="I5" s="19">
+        <v>41583</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="24" t="s">
@@ -4169,6 +4187,24 @@
       </c>
       <c r="F7">
         <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B14" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B24" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -4181,7 +4217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
US30, Tests, and Updated Excel
</commit_message>
<xml_diff>
--- a/khrwhjvtReport.xlsx
+++ b/khrwhjvtReport.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Harish7KJ/Desktop/ssw555-master-7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rweis\OneDrive\Stevens\SSW 555 - Agile\ssw555\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="9" documentId="F8F5781F81411D2690ADB5D578A1944668529B6B" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{E9C72E0D-733C-4253-A3CB-BAF38FDEBBE9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="463" windowWidth="23451" windowHeight="11914" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="217">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -721,7 +722,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1020,7 +1021,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1046,13 +1047,13 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41542.0</c:v>
+                  <c:v>41542</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41548.0</c:v>
+                  <c:v>41548</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1064,25 +1065,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5795-419D-BE09-C3BBDA1361DE}"/>
             </c:ext>
@@ -1108,7 +1109,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1141,14 +1142,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1174,16 +1175,16 @@
             <c:numRef>
               <c:f>Burndown!$A$2:$A$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41542.0</c:v>
+                  <c:v>41542</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41548.0</c:v>
+                  <c:v>41548</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="m/d">
-                  <c:v>41575.0</c:v>
+                  <c:v>41575</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1195,19 +1196,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2CBE-44F9-A43F-F19DA2381D0D}"/>
             </c:ext>
@@ -1233,7 +1234,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1266,7 +1267,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1292,7 +1293,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1330,7 +1331,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1405,7 +1406,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1470,7 +1471,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1539,7 +1540,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1609,7 +1610,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1678,7 +1679,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1748,7 +1749,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2088,22 +2089,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="165" zoomScaleNormal="165" zoomScalePageLayoutView="165" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="4" max="5" width="20.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2120,7 +2121,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -2137,7 +2138,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>183</v>
       </c>
@@ -2154,7 +2155,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>194</v>
       </c>
@@ -2171,7 +2172,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>195</v>
       </c>
@@ -2188,7 +2189,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2202,10 +2203,10 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2213,14 +2214,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A16" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" customWidth="1"/>
@@ -2229,7 +2230,7 @@
     <col min="5" max="5" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2246,7 +2247,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2263,7 +2264,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2277,7 +2278,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2291,7 +2292,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2305,7 +2306,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2322,7 +2323,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2339,7 +2340,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2353,7 +2354,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2367,7 +2368,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2381,7 +2382,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2395,7 +2396,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>124</v>
       </c>
@@ -2406,7 +2407,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>125</v>
       </c>
@@ -2417,7 +2418,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2431,7 +2432,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2445,7 +2446,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2462,7 +2463,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>129</v>
       </c>
@@ -2473,7 +2474,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>130</v>
       </c>
@@ -2484,7 +2485,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>131</v>
       </c>
@@ -2495,7 +2496,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>132</v>
       </c>
@@ -2506,7 +2507,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>133</v>
       </c>
@@ -2517,7 +2518,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2534,7 +2535,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2551,7 +2552,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2565,7 +2566,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>137</v>
       </c>
@@ -2576,7 +2577,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2590,7 +2591,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>139</v>
       </c>
@@ -2601,7 +2602,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
@@ -2615,7 +2616,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -2629,7 +2630,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -2643,18 +2644,24 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>4</v>
+      </c>
       <c r="B31" t="s">
         <v>143</v>
       </c>
       <c r="C31" t="s">
         <v>99</v>
       </c>
+      <c r="D31" t="s">
+        <v>183</v>
+      </c>
       <c r="E31" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2668,7 +2675,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>145</v>
       </c>
@@ -2679,7 +2686,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2693,7 +2700,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2715,54 +2722,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="150" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="9.46484375" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="6" max="6" width="12.46484375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>162</v>
       </c>
@@ -2785,7 +2792,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>163</v>
       </c>
@@ -2804,7 +2811,7 @@
       <c r="F15" s="13"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -2829,7 +2836,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>165</v>
       </c>
@@ -2845,7 +2852,7 @@
       <c r="F17" s="14"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>166</v>
       </c>
@@ -2861,7 +2868,7 @@
       <c r="F18" s="14"/>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>167</v>
       </c>
@@ -2885,23 +2892,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="18.1328125" customWidth="1"/>
+    <col min="3" max="3" width="12.46484375" customWidth="1"/>
     <col min="4" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="6" max="6" width="12.46484375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2921,7 +2928,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>41542</v>
       </c>
@@ -2942,7 +2949,7 @@
         <v>18.715596330275229</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>41548</v>
       </c>
@@ -2963,7 +2970,7 @@
         <v>18.830769230769231</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>41575</v>
       </c>
@@ -2992,26 +2999,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.46484375" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="7.5" customWidth="1"/>
+    <col min="6" max="6" width="7.46484375" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" customWidth="1"/>
     <col min="8" max="8" width="7.6640625" customWidth="1"/>
     <col min="9" max="9" width="11" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3040,7 +3047,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3069,7 +3076,7 @@
         <v>41542</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -3098,7 +3105,7 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3127,7 +3134,7 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3156,7 +3163,7 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3185,7 +3192,7 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -3214,7 +3221,7 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3243,7 +3250,7 @@
         <v>41542</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3272,7 +3279,7 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3301,7 +3308,7 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G11">
         <f>SUM(G2:G10)</f>
         <v>170</v>
@@ -3311,51 +3318,51 @@
         <v>545</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="26" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>204</v>
       </c>
@@ -3368,19 +3375,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3409,7 +3416,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -3438,7 +3445,7 @@
         <v>41556</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -3467,7 +3474,7 @@
         <v>41562</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -3496,7 +3503,7 @@
         <v>41562</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -3525,7 +3532,7 @@
         <v>41562</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -3554,7 +3561,7 @@
         <v>41562</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -3583,7 +3590,7 @@
         <v>41562</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -3612,60 +3619,60 @@
         <v>41562</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="26" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="26" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>204</v>
       </c>
@@ -3678,21 +3685,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="23"/>
-    <col min="2" max="2" width="26.83203125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="26.796875" style="23" customWidth="1"/>
     <col min="3" max="16384" width="11" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>3</v>
       </c>
@@ -3721,7 +3728,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>134</v>
       </c>
@@ -3750,7 +3757,7 @@
         <v>41571</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>135</v>
       </c>
@@ -3779,7 +3786,7 @@
         <v>41575</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
         <v>136</v>
       </c>
@@ -3808,7 +3815,7 @@
         <v>41575</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>138</v>
       </c>
@@ -3837,7 +3844,7 @@
         <v>41575</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>144</v>
       </c>
@@ -3866,7 +3873,7 @@
         <v>41576</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
         <v>148</v>
       </c>
@@ -3895,7 +3902,7 @@
         <v>41576</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>146</v>
       </c>
@@ -3915,7 +3922,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>147</v>
       </c>
@@ -3935,70 +3942,70 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="26" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="26" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="26" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="26" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="31" t="s">
         <v>216</v>
       </c>
@@ -4010,19 +4017,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4051,7 +4058,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>155</v>
       </c>
@@ -4071,7 +4078,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -4090,8 +4097,17 @@
       <c r="F3">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+      <c r="I3" s="19">
+        <v>41588</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -4120,7 +4136,7 @@
         <v>41583</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>151</v>
       </c>
@@ -4149,7 +4165,7 @@
         <v>41583</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>129</v>
       </c>
@@ -4169,7 +4185,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>145</v>
       </c>
@@ -4189,20 +4205,20 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>32</v>
       </c>
@@ -4214,22 +4230,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A38" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="27"/>
     <col min="2" max="2" width="28" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="29" customWidth="1"/>
+    <col min="3" max="3" width="49.46484375" style="29" customWidth="1"/>
     <col min="4" max="16384" width="11" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>113</v>
       </c>
@@ -4240,7 +4256,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>114</v>
       </c>
@@ -4251,7 +4267,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>115</v>
       </c>
@@ -4262,7 +4278,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>116</v>
       </c>
@@ -4273,7 +4289,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>117</v>
       </c>
@@ -4284,7 +4300,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>118</v>
       </c>
@@ -4295,7 +4311,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>119</v>
       </c>
@@ -4306,7 +4322,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
         <v>120</v>
       </c>
@@ -4317,7 +4333,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>121</v>
       </c>
@@ -4328,7 +4344,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>122</v>
       </c>
@@ -4339,7 +4355,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>123</v>
       </c>
@@ -4350,7 +4366,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
         <v>124</v>
       </c>
@@ -4361,7 +4377,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
         <v>125</v>
       </c>
@@ -4372,7 +4388,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="64" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
         <v>126</v>
       </c>
@@ -4383,7 +4399,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>127</v>
       </c>
@@ -4394,7 +4410,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
         <v>128</v>
       </c>
@@ -4405,7 +4421,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>129</v>
       </c>
@@ -4416,7 +4432,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>130</v>
       </c>
@@ -4427,7 +4443,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>131</v>
       </c>
@@ -4438,7 +4454,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
         <v>132</v>
       </c>
@@ -4449,7 +4465,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
         <v>133</v>
       </c>
@@ -4460,7 +4476,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>134</v>
       </c>
@@ -4471,7 +4487,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
         <v>135</v>
       </c>
@@ -4482,7 +4498,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
         <v>136</v>
       </c>
@@ -4493,7 +4509,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="s">
         <v>137</v>
       </c>
@@ -4504,7 +4520,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
         <v>138</v>
       </c>
@@ -4515,7 +4531,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="128" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
         <v>139</v>
       </c>
@@ -4526,7 +4542,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
         <v>140</v>
       </c>
@@ -4537,7 +4553,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
         <v>141</v>
       </c>
@@ -4548,7 +4564,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
         <v>142</v>
       </c>
@@ -4559,7 +4575,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" s="27" t="s">
         <v>143</v>
       </c>
@@ -4570,7 +4586,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" s="27" t="s">
         <v>144</v>
       </c>
@@ -4581,7 +4597,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" s="27" t="s">
         <v>145</v>
       </c>
@@ -4592,7 +4608,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" s="27" t="s">
         <v>146</v>
       </c>
@@ -4603,7 +4619,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
         <v>147</v>
       </c>
@@ -4614,7 +4630,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
         <v>148</v>
       </c>
@@ -4625,7 +4641,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
         <v>149</v>
       </c>
@@ -4636,7 +4652,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A38" s="27" t="s">
         <v>150</v>
       </c>
@@ -4647,7 +4663,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" s="27" t="s">
         <v>151</v>
       </c>
@@ -4658,7 +4674,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A40" s="27" t="s">
         <v>152</v>
       </c>
@@ -4669,7 +4685,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" s="27" t="s">
         <v>153</v>
       </c>
@@ -4680,7 +4696,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" s="27" t="s">
         <v>154</v>
       </c>
@@ -4691,7 +4707,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" s="27" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
US42, Tests, Updated Excel
</commit_message>
<xml_diff>
--- a/khrwhjvtReport.xlsx
+++ b/khrwhjvtReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rweis\OneDrive\Stevens\SSW 555 - Agile\ssw555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="F8F5781F81411D2690ADB5D578A1944668529B6B" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{E9C72E0D-733C-4253-A3CB-BAF38FDEBBE9}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="F8F5781F81411D2690ADB5D578A1944668529B6B" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{1B53F71A-D6F0-4B35-828C-7B38037F0927}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="463" windowWidth="23451" windowHeight="11914" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="463" windowWidth="23451" windowHeight="11914" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="217">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2215,10 +2215,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -2712,6 +2712,23 @@
       </c>
       <c r="E35" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" t="s">
+        <v>183</v>
+      </c>
+      <c r="E36" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -4020,8 +4037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -4076,6 +4093,15 @@
       </c>
       <c r="F2">
         <v>60</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>50</v>
+      </c>
+      <c r="I2" s="19">
+        <v>41588</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -4234,7 +4260,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView topLeftCell="A38" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:C43"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated Excel and user stories
</commit_message>
<xml_diff>
--- a/khrwhjvtReport.xlsx
+++ b/khrwhjvtReport.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rweis\OneDrive\Stevens\SSW 555 - Agile\ssw555\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slyst\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="F8F5781F81411D2690ADB5D578A1944668529B6B" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{1B53F71A-D6F0-4B35-828C-7B38037F0927}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="463" windowWidth="23451" windowHeight="11914" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="6696" tabRatio="500" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="218">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -717,12 +716,15 @@
   </si>
   <si>
     <t>Writing bad unit tests</t>
+  </si>
+  <si>
+    <t>List recent Aniversarries</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2089,22 +2091,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="165" zoomScaleNormal="165" zoomScalePageLayoutView="165" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="5" width="20.46484375" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="10.36328125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2121,7 +2123,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -2138,7 +2140,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>183</v>
       </c>
@@ -2155,7 +2157,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>194</v>
       </c>
@@ -2172,7 +2174,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>195</v>
       </c>
@@ -2189,7 +2191,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2203,10 +2205,10 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2214,23 +2216,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.36328125" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2247,7 +2249,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2264,7 +2266,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2278,7 +2280,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2292,7 +2294,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2306,7 +2308,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2323,7 +2325,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2340,7 +2342,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2354,7 +2356,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2368,7 +2370,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2382,7 +2384,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2396,7 +2398,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>124</v>
       </c>
@@ -2407,7 +2409,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>125</v>
       </c>
@@ -2418,7 +2420,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2432,7 +2434,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2446,7 +2448,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2463,7 +2465,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>129</v>
       </c>
@@ -2474,7 +2476,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>130</v>
       </c>
@@ -2485,7 +2487,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>131</v>
       </c>
@@ -2496,7 +2498,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>132</v>
       </c>
@@ -2507,7 +2509,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>133</v>
       </c>
@@ -2518,7 +2520,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2535,7 +2537,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2552,7 +2554,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2566,7 +2568,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>137</v>
       </c>
@@ -2577,7 +2579,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2591,7 +2593,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>139</v>
       </c>
@@ -2602,7 +2604,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -2616,7 +2618,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -2630,7 +2632,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -2644,7 +2646,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2661,7 +2663,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2675,7 +2677,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>145</v>
       </c>
@@ -2686,7 +2688,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2700,7 +2702,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2714,7 +2716,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2739,54 +2741,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="150" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="7"/>
-    <col min="2" max="2" width="9.46484375" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="12.46484375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>162</v>
       </c>
@@ -2809,7 +2811,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>163</v>
       </c>
@@ -2828,7 +2830,7 @@
       <c r="F15" s="13"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -2853,7 +2855,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>165</v>
       </c>
@@ -2869,7 +2871,7 @@
       <c r="F17" s="14"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>166</v>
       </c>
@@ -2885,7 +2887,7 @@
       <c r="F18" s="14"/>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>167</v>
       </c>
@@ -2909,23 +2911,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
-    <col min="2" max="2" width="18.1328125" customWidth="1"/>
-    <col min="3" max="3" width="12.46484375" customWidth="1"/>
+    <col min="2" max="2" width="18.08984375" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
     <col min="4" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="12.46484375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2945,7 +2947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
         <v>41542</v>
       </c>
@@ -2966,7 +2968,7 @@
         <v>18.715596330275229</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>41548</v>
       </c>
@@ -2987,7 +2989,7 @@
         <v>18.830769230769231</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>41575</v>
       </c>
@@ -3016,26 +3018,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.46484375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="7.46484375" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="7.453125" customWidth="1"/>
+    <col min="7" max="7" width="6.6328125" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" customWidth="1"/>
     <col min="9" max="9" width="11" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3064,7 +3066,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3093,7 +3095,7 @@
         <v>41542</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -3122,7 +3124,7 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3151,7 +3153,7 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3180,7 +3182,7 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3209,7 +3211,7 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -3238,7 +3240,7 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3267,7 +3269,7 @@
         <v>41542</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3296,7 +3298,7 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3325,7 +3327,7 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G11">
         <f>SUM(G2:G10)</f>
         <v>170</v>
@@ -3335,51 +3337,51 @@
         <v>545</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>204</v>
       </c>
@@ -3392,19 +3394,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3433,7 +3435,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -3462,7 +3464,7 @@
         <v>41556</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -3491,7 +3493,7 @@
         <v>41562</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -3520,7 +3522,7 @@
         <v>41562</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -3549,7 +3551,7 @@
         <v>41562</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -3578,7 +3580,7 @@
         <v>41562</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -3607,7 +3609,7 @@
         <v>41562</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -3636,60 +3638,60 @@
         <v>41562</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>204</v>
       </c>
@@ -3702,21 +3704,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="23"/>
-    <col min="2" max="2" width="26.796875" style="23" customWidth="1"/>
+    <col min="2" max="2" width="26.81640625" style="23" customWidth="1"/>
     <col min="3" max="16384" width="11" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>3</v>
       </c>
@@ -3745,7 +3747,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>134</v>
       </c>
@@ -3774,7 +3776,7 @@
         <v>41571</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>135</v>
       </c>
@@ -3803,7 +3805,7 @@
         <v>41575</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>136</v>
       </c>
@@ -3832,7 +3834,7 @@
         <v>41575</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>138</v>
       </c>
@@ -3861,7 +3863,7 @@
         <v>41575</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
         <v>144</v>
       </c>
@@ -3890,7 +3892,7 @@
         <v>41576</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
         <v>148</v>
       </c>
@@ -3919,7 +3921,7 @@
         <v>41576</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
         <v>146</v>
       </c>
@@ -3939,7 +3941,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>147</v>
       </c>
@@ -3959,70 +3961,70 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" s="31" t="s">
         <v>216</v>
       </c>
@@ -4034,19 +4036,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4075,7 +4077,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>155</v>
       </c>
@@ -4104,7 +4106,7 @@
         <v>41588</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -4133,7 +4135,7 @@
         <v>41588</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -4162,7 +4164,7 @@
         <v>41583</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>151</v>
       </c>
@@ -4191,7 +4193,7 @@
         <v>41583</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
         <v>129</v>
       </c>
@@ -4211,7 +4213,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>145</v>
       </c>
@@ -4231,20 +4233,83 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>15</v>
+      </c>
+      <c r="I9" s="19">
+        <v>41590</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>30</v>
+      </c>
+      <c r="G10">
+        <v>15</v>
+      </c>
+      <c r="H10">
+        <v>40</v>
+      </c>
+      <c r="I10" s="19">
+        <v>41590</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>32</v>
       </c>
@@ -4256,22 +4321,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="27"/>
     <col min="2" max="2" width="28" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.46484375" style="29" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="29" customWidth="1"/>
     <col min="4" max="16384" width="11" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>113</v>
       </c>
@@ -4282,7 +4347,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>114</v>
       </c>
@@ -4293,7 +4358,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>115</v>
       </c>
@@ -4304,7 +4369,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
         <v>116</v>
       </c>
@@ -4315,7 +4380,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>117</v>
       </c>
@@ -4326,7 +4391,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
         <v>118</v>
       </c>
@@ -4337,7 +4402,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>119</v>
       </c>
@@ -4348,7 +4413,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
         <v>120</v>
       </c>
@@ -4359,7 +4424,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
         <v>121</v>
       </c>
@@ -4370,7 +4435,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>122</v>
       </c>
@@ -4381,7 +4446,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
         <v>123</v>
       </c>
@@ -4392,7 +4457,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
         <v>124</v>
       </c>
@@ -4403,7 +4468,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
         <v>125</v>
       </c>
@@ -4414,7 +4479,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
         <v>126</v>
       </c>
@@ -4425,7 +4490,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
         <v>127</v>
       </c>
@@ -4436,7 +4501,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
         <v>128</v>
       </c>
@@ -4447,7 +4512,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
         <v>129</v>
       </c>
@@ -4458,7 +4523,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
         <v>130</v>
       </c>
@@ -4469,7 +4534,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
         <v>131</v>
       </c>
@@ -4480,7 +4545,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="s">
         <v>132</v>
       </c>
@@ -4491,7 +4556,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
         <v>133</v>
       </c>
@@ -4502,7 +4567,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
         <v>134</v>
       </c>
@@ -4513,7 +4578,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="27" t="s">
         <v>135</v>
       </c>
@@ -4524,7 +4589,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
         <v>136</v>
       </c>
@@ -4535,7 +4600,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="27" t="s">
         <v>137</v>
       </c>
@@ -4546,7 +4611,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="27" t="s">
         <v>138</v>
       </c>
@@ -4557,7 +4622,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" s="27" t="s">
         <v>139</v>
       </c>
@@ -4568,7 +4633,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="s">
         <v>140</v>
       </c>
@@ -4579,7 +4644,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="27" t="s">
         <v>141</v>
       </c>
@@ -4590,7 +4655,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="27" t="s">
         <v>142</v>
       </c>
@@ -4601,7 +4666,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="27" t="s">
         <v>143</v>
       </c>
@@ -4612,7 +4677,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="27" t="s">
         <v>144</v>
       </c>
@@ -4623,7 +4688,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="27" t="s">
         <v>145</v>
       </c>
@@ -4634,7 +4699,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="27" t="s">
         <v>146</v>
       </c>
@@ -4645,7 +4710,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="27" t="s">
         <v>147</v>
       </c>
@@ -4656,7 +4721,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="27" t="s">
         <v>148</v>
       </c>
@@ -4667,7 +4732,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="27" t="s">
         <v>149</v>
       </c>
@@ -4678,7 +4743,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="27" t="s">
         <v>150</v>
       </c>
@@ -4689,7 +4754,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="27" t="s">
         <v>151</v>
       </c>
@@ -4700,7 +4765,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="27" t="s">
         <v>152</v>
       </c>
@@ -4711,7 +4776,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="27" t="s">
         <v>153</v>
       </c>
@@ -4722,7 +4787,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="27" t="s">
         <v>154</v>
       </c>
@@ -4733,7 +4798,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="27" t="s">
         <v>155</v>
       </c>

</xml_diff>